<commit_message>
Descrição do tipo de impacto para IOPC + Coluna de tipo de impacto geral na tabela final
</commit_message>
<xml_diff>
--- a/docs/df_jusbrasil_iopc.xlsx
+++ b/docs/df_jusbrasil_iopc.xlsx
@@ -8973,12 +8973,12 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -9088,12 +9088,12 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N82" t="inlineStr">
@@ -9203,12 +9203,12 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N83" t="inlineStr">
@@ -9318,12 +9318,12 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -9433,12 +9433,12 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
@@ -9548,12 +9548,12 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -9663,12 +9663,12 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -9778,12 +9778,12 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -9893,12 +9893,12 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
@@ -10008,12 +10008,12 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N90" t="inlineStr">
@@ -10123,12 +10123,12 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
@@ -10238,12 +10238,12 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
@@ -10353,12 +10353,12 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -10468,12 +10468,12 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
@@ -10583,12 +10583,12 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
@@ -10698,12 +10698,12 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
@@ -10813,12 +10813,12 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
@@ -10928,12 +10928,12 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N98" t="inlineStr">
@@ -11043,12 +11043,12 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
@@ -11158,12 +11158,12 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N100" t="inlineStr">
@@ -11273,12 +11273,12 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
@@ -11388,12 +11388,12 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N102" t="inlineStr">
@@ -11503,12 +11503,12 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N103" t="inlineStr">
@@ -11618,12 +11618,12 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N104" t="inlineStr">
@@ -11733,12 +11733,12 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -11848,12 +11848,12 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -11963,12 +11963,12 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N107" t="inlineStr">
@@ -12078,12 +12078,12 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -12193,12 +12193,12 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -12308,12 +12308,12 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N110" t="inlineStr">
@@ -12423,12 +12423,12 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -12538,12 +12538,12 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
@@ -12653,12 +12653,12 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -12768,12 +12768,12 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
@@ -12883,12 +12883,12 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
@@ -12998,12 +12998,12 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
@@ -13113,12 +13113,12 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
@@ -13228,12 +13228,12 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -13343,12 +13343,12 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N119" t="inlineStr">
@@ -13458,12 +13458,12 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N120" t="inlineStr">
@@ -13573,12 +13573,12 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
@@ -13688,12 +13688,12 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N122" t="inlineStr">
@@ -13803,12 +13803,12 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N123" t="inlineStr">
@@ -13918,12 +13918,12 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
@@ -14033,12 +14033,12 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -14148,12 +14148,12 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N126" t="inlineStr">
@@ -14263,12 +14263,12 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
@@ -14378,12 +14378,12 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N128" t="inlineStr">
@@ -14493,12 +14493,12 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N129" t="inlineStr">
@@ -14608,12 +14608,12 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -14723,12 +14723,12 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
@@ -14838,12 +14838,12 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -14953,12 +14953,12 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N133" t="inlineStr">
@@ -15068,12 +15068,12 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N134" t="inlineStr">
@@ -15183,12 +15183,12 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
@@ -15298,12 +15298,12 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
@@ -15413,12 +15413,12 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N137" t="inlineStr">
@@ -15528,12 +15528,12 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N138" t="inlineStr">
@@ -15643,12 +15643,12 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
@@ -15758,12 +15758,12 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
@@ -15873,12 +15873,12 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N141" t="inlineStr">
@@ -15988,12 +15988,12 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N142" t="inlineStr">
@@ -16103,12 +16103,12 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N143" t="inlineStr">
@@ -16218,12 +16218,12 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M144" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N144" t="inlineStr">
@@ -16333,12 +16333,12 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N145" t="inlineStr">
@@ -16448,12 +16448,12 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N146" t="inlineStr">
@@ -16563,12 +16563,12 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N147" t="inlineStr">
@@ -16678,12 +16678,12 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N148" t="inlineStr">
@@ -16793,12 +16793,12 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N149" t="inlineStr">
@@ -16908,12 +16908,12 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Derramamento de petróleo</t>
         </is>
       </c>
       <c r="N150" t="inlineStr">

</xml_diff>